<commit_message>
ajout des docs mis à jour
</commit_message>
<xml_diff>
--- a/Docs/diag_Gatt_prevision.xlsx
+++ b/Docs/diag_Gatt_prevision.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\iutbg-smbetu.univ-lyon1.fr\homes\Documents\SAE 203\pong\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\SAE 203\pong\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C099B1-1F24-4447-9CA5-7DB76AB443D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4630605-8ECF-4DFD-83A3-D408769C5C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB7587E1-D77B-4CEA-BE79-96ECA762180D}"/>
+    <workbookView xWindow="17220" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{BB7587E1-D77B-4CEA-BE79-96ECA762180D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -683,7 +683,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>